<commit_message>
added/verified pulp bleaching unit
</commit_message>
<xml_diff>
--- a/data/paper/paper_calc.xlsx
+++ b/data/paper/paper_calc.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\BlackBlox\data\paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0D0D94-989D-0F4B-8488-4A476A884DF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25410" windowHeight="13350" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25420" windowHeight="13360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -22,17 +23,23 @@
     <sheet name="Caustic" sheetId="9" r:id="rId8"/>
     <sheet name="Board" sheetId="6" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="102">
   <si>
     <t>meta-process</t>
   </si>
@@ -281,12 +288,69 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>bleached pulp</t>
+  </si>
+  <si>
+    <t>pulp ratio</t>
+  </si>
+  <si>
+    <t>washing water</t>
+  </si>
+  <si>
+    <t>washing water demand</t>
+  </si>
+  <si>
+    <t>NaOH</t>
+  </si>
+  <si>
+    <t>NaOH demand</t>
+  </si>
+  <si>
+    <t>H2O2</t>
+  </si>
+  <si>
+    <t>Talc</t>
+  </si>
+  <si>
+    <t>NaCl3</t>
+  </si>
+  <si>
+    <t>H2SO4</t>
+  </si>
+  <si>
+    <t>Methanol</t>
+  </si>
+  <si>
+    <t>filter cake</t>
+  </si>
+  <si>
+    <t>filter cake ratio</t>
+  </si>
+  <si>
+    <t>Methanol demand</t>
+  </si>
+  <si>
+    <t>H2O2 demand</t>
+  </si>
+  <si>
+    <t>Talc demand</t>
+  </si>
+  <si>
+    <t>NaCl3 demand</t>
+  </si>
+  <si>
+    <t>H2SO4 demand</t>
+  </si>
+  <si>
+    <t>effluent ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -344,7 +408,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -621,16 +685,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,7 +726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -688,7 +752,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>11</v>
@@ -712,7 +776,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -724,7 +788,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -747,7 +811,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
@@ -764,7 +828,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -784,7 +848,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>24</v>
@@ -802,10 +866,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
@@ -828,7 +892,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="5" t="s">
         <v>27</v>
@@ -847,7 +911,7 @@
       </c>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -856,7 +920,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -879,14 +943,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
@@ -910,7 +974,7 @@
       </c>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="5" t="s">
         <v>38</v>
@@ -932,7 +996,7 @@
       </c>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="B18" s="5" t="s">
         <v>38</v>
@@ -954,7 +1018,7 @@
       </c>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="5" t="s">
         <v>43</v>
@@ -974,7 +1038,7 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="5" t="s">
         <v>44</v>
@@ -994,7 +1058,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>45</v>
       </c>
@@ -1020,7 +1084,7 @@
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="5" t="s">
         <v>46</v>
@@ -1042,7 +1106,7 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="5" t="s">
         <v>47</v>
@@ -1066,7 +1130,7 @@
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="5" t="s">
         <v>47</v>
@@ -1090,7 +1154,7 @@
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="B26" s="5" t="s">
         <v>43</v>
@@ -1112,7 +1176,7 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="5" t="s">
         <v>44</v>
@@ -1134,7 +1198,7 @@
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>49</v>
       </c>
@@ -1154,7 +1218,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="6" t="s">
         <v>50</v>
@@ -1178,27 +1242,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1230,7 +1294,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>57</v>
       </c>
@@ -1250,7 +1314,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>57</v>
       </c>
@@ -1270,7 +1334,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>60</v>
       </c>
@@ -1290,7 +1354,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>60</v>
       </c>
@@ -1310,7 +1374,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>56</v>
       </c>
@@ -1330,7 +1394,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>63</v>
       </c>
@@ -1353,7 +1417,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>56</v>
       </c>
@@ -1373,7 +1437,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -1396,27 +1460,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1448,7 +1512,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>56</v>
       </c>
@@ -1468,7 +1532,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>56</v>
       </c>
@@ -1488,7 +1552,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>56</v>
       </c>
@@ -1508,7 +1572,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>67</v>
       </c>
@@ -1528,7 +1592,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>67</v>
       </c>
@@ -1548,7 +1612,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>67</v>
       </c>
@@ -1568,7 +1632,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>67</v>
       </c>
@@ -1588,7 +1652,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>67</v>
       </c>
@@ -1608,7 +1672,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>67</v>
       </c>
@@ -1628,7 +1692,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>19</v>
       </c>
@@ -1645,7 +1709,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J24" t="s">
         <v>82</v>
       </c>
@@ -1656,26 +1720,360 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1712,27 +2110,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1769,27 +2167,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1826,84 +2224,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1941,26 +2282,26 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>